<commit_message>
ng: update lf forms
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Nigeria/apri 2024/ng_lf_pretas_202404_1_site.xlsx
+++ b/LF/PreTAS/Nigeria/apri 2024/ng_lf_pretas_202404_1_site.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\PreTAS\Nigeria\apri 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CAA8E3F-9681-4BEB-BBD0-51650B7D5C36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EBE882-FDCF-4433-8D94-F59227C7E7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="163">
   <si>
     <t>type</t>
   </si>
@@ -89,12 +89,6 @@
     <t>If you are the only recorder on your team, this may be called a "team ID". Recorder ID is the 2-digit code assigned to you or your team.</t>
   </si>
   <si>
-    <t>. &gt; 9 and . &lt; 100</t>
-  </si>
-  <si>
-    <t>The code must be a two-digit number between 9 and 100</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -122,9 +116,6 @@
     <t>c_cluster_name</t>
   </si>
   <si>
-    <t>Select the site</t>
-  </si>
-  <si>
     <t>district = ${c_district}</t>
   </si>
   <si>
@@ -134,9 +125,6 @@
     <t>c_site_type</t>
   </si>
   <si>
-    <t>Select the site type</t>
-  </si>
-  <si>
     <t>site_liste= ${c_cluster_name}</t>
   </si>
   <si>
@@ -161,18 +149,12 @@
     <t>c_cluster_leader</t>
   </si>
   <si>
-    <t>Name of Village Leader or Head Teacher</t>
-  </si>
-  <si>
     <t>select_one yes_no</t>
   </si>
   <si>
     <t>c_consent</t>
   </si>
   <si>
-    <t>Does the school leader or community leader consent to participating in this survey?</t>
-  </si>
-  <si>
     <t>geopoint</t>
   </si>
   <si>
@@ -377,9 +359,6 @@
     <t>begin group</t>
   </si>
   <si>
-    <t>ng_lf_pretas_202404_1_site</t>
-  </si>
-  <si>
     <t>Sentinel Site</t>
   </si>
   <si>
@@ -509,7 +488,43 @@
     <t>Code Site</t>
   </si>
   <si>
-    <t>(Apr 2024) - 1. Nigeria - Pre TAS LF Site Form</t>
+    <t>(Apr 2024) - 1. Nigeria - Pre TAS LF Site Form V2</t>
+  </si>
+  <si>
+    <t>ng_lf_pretas_202404_1_site_v2</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>99</t>
+  </si>
+  <si>
+    <t>select_one team</t>
+  </si>
+  <si>
+    <t>Name of Village Leader</t>
+  </si>
+  <si>
+    <t>Does the community leader consent to participating in this survey?</t>
+  </si>
+  <si>
+    <t>Select the community</t>
+  </si>
+  <si>
+    <t>Select the community type</t>
   </si>
 </sst>
 </file>
@@ -626,7 +641,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -673,6 +688,9 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1030,7 +1048,7 @@
     </row>
     <row r="2" spans="1:13" s="9" customFormat="1" ht="47.25">
       <c r="A2" s="9" t="s">
-        <v>13</v>
+        <v>158</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>14</v>
@@ -1042,16 +1060,11 @@
         <v>16</v>
       </c>
       <c r="E2" s="14"/>
-      <c r="F2" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>18</v>
-      </c>
+      <c r="G2" s="14"/>
       <c r="H2" s="14"/>
       <c r="I2" s="14"/>
       <c r="J2" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K2" s="14"/>
       <c r="L2" s="14"/>
@@ -1059,130 +1072,130 @@
     </row>
     <row r="3" spans="1:13" s="9" customFormat="1">
       <c r="A3" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="14" t="s">
         <v>20</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>22</v>
       </c>
       <c r="D3" s="14"/>
       <c r="G3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K3" s="14"/>
       <c r="L3" s="14"/>
     </row>
     <row r="4" spans="1:13" s="9" customFormat="1">
       <c r="A4" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D4" s="14"/>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="14"/>
       <c r="J4" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K4" s="14"/>
       <c r="L4" s="14"/>
       <c r="M4" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="9" customFormat="1">
       <c r="A5" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="14" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>28</v>
+        <v>161</v>
       </c>
       <c r="D5" s="14"/>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K5" s="14"/>
       <c r="L5" s="14"/>
       <c r="M5" s="14" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="9" customFormat="1">
       <c r="A6" s="9" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>32</v>
+        <v>162</v>
       </c>
       <c r="D6" s="14"/>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K6" s="14"/>
       <c r="L6" s="14"/>
       <c r="M6" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="9" customFormat="1" ht="31.5">
       <c r="A7" s="9" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="14"/>
       <c r="F7" s="9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G7" s="14" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K7" s="14"/>
       <c r="L7" s="14"/>
       <c r="M7" s="14" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="9" customFormat="1" ht="15.75" customHeight="1">
       <c r="A8" s="9" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>41</v>
+        <v>159</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1191,7 +1204,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K8" s="14"/>
       <c r="L8" s="14"/>
@@ -1199,17 +1212,17 @@
     </row>
     <row r="9" spans="1:13" s="9" customFormat="1" ht="31.5">
       <c r="A9" s="9" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>44</v>
+        <v>160</v>
       </c>
       <c r="D9" s="14"/>
       <c r="J9" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="9" customFormat="1">
@@ -1217,20 +1230,20 @@
         <v>13</v>
       </c>
       <c r="B10" s="14" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="14"/>
       <c r="G10" s="14"/>
       <c r="H10" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="I10" s="14"/>
       <c r="J10" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
@@ -1238,82 +1251,82 @@
     </row>
     <row r="11" spans="1:13" s="9" customFormat="1" ht="31.5">
       <c r="A11" s="9" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B11" s="14" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="D11" s="14" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="9" customFormat="1">
       <c r="A12" s="9" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="9" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="H12" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J12" s="14"/>
     </row>
     <row r="13" spans="1:13" s="9" customFormat="1">
       <c r="A13" s="9" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="D13" s="14"/>
       <c r="H13" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J13" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="9" customFormat="1">
       <c r="A14" s="9" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="B14" s="14" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="D14" s="14"/>
       <c r="H14" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J14" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="8" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="16" spans="1:13">
@@ -1321,16 +1334,16 @@
         <v>13</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="H16" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J16" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:10">
@@ -1338,67 +1351,67 @@
         <v>13</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="H17" s="9" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="J17" s="14" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="9" customFormat="1">
       <c r="A18" s="9" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B18" s="14" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D18" s="14"/>
       <c r="H18" s="9" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="J18" s="14"/>
     </row>
     <row r="19" spans="1:10" s="9" customFormat="1">
       <c r="A19" s="9" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B19" s="14" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:10" s="9" customFormat="1">
       <c r="A20" s="9" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:10" s="9" customFormat="1">
       <c r="A21" s="9" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D21" s="14"/>
     </row>
@@ -1410,11 +1423,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B128" sqref="B128"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A11" sqref="A6:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1426,7 +1439,7 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="2" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
@@ -1435,1661 +1448,1722 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" s="8" customFormat="1">
-      <c r="A2" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>87</v>
-      </c>
-      <c r="F2" s="14"/>
-    </row>
-    <row r="3" spans="1:6" s="8" customFormat="1">
-      <c r="A3" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="F3" s="14"/>
-    </row>
-    <row r="4" spans="1:6" s="8" customFormat="1">
-      <c r="A4" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="F4" s="14"/>
-    </row>
-    <row r="5" spans="1:6" s="8" customFormat="1">
-      <c r="A5" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>90</v>
-      </c>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="1:6" s="8" customFormat="1">
-      <c r="A6" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="F6" s="14"/>
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" s="4" customFormat="1">
+      <c r="A2" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>153</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="4" customFormat="1">
+      <c r="A3" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" s="4" customFormat="1">
+      <c r="A4" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="4" customFormat="1">
+      <c r="A5" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="4" customFormat="1">
+      <c r="A6" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="7" spans="1:6" s="8" customFormat="1">
-      <c r="A7" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>92</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>92</v>
-      </c>
+      <c r="A7" s="9"/>
+      <c r="B7" s="9"/>
+      <c r="C7" s="9"/>
       <c r="F7" s="14"/>
     </row>
     <row r="8" spans="1:6" s="8" customFormat="1">
       <c r="A8" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B8" s="9" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="F8" s="14"/>
     </row>
     <row r="9" spans="1:6" s="8" customFormat="1">
       <c r="A9" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="F9" s="14"/>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1">
       <c r="A10" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F10" s="14"/>
     </row>
     <row r="11" spans="1:6" s="8" customFormat="1">
       <c r="A11" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="F11" s="14"/>
     </row>
     <row r="12" spans="1:6" s="8" customFormat="1">
       <c r="A12" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" s="8" customFormat="1">
       <c r="A13" s="9" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:6" s="8" customFormat="1">
       <c r="A14" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B14" s="9">
-        <v>2000</v>
-      </c>
-      <c r="C14" s="9">
-        <v>2000</v>
+        <v>93</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>87</v>
       </c>
       <c r="F14" s="14"/>
     </row>
     <row r="15" spans="1:6" s="8" customFormat="1">
       <c r="A15" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="9">
-        <v>2001</v>
-      </c>
-      <c r="C15" s="9">
-        <v>2001</v>
+        <v>93</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>88</v>
       </c>
       <c r="F15" s="14"/>
     </row>
     <row r="16" spans="1:6" s="8" customFormat="1">
       <c r="A16" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B16" s="9">
-        <v>2002</v>
-      </c>
-      <c r="C16" s="9">
-        <v>2002</v>
+        <v>93</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>89</v>
       </c>
       <c r="F16" s="14"/>
     </row>
     <row r="17" spans="1:6" s="8" customFormat="1">
       <c r="A17" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B17" s="9">
-        <v>2003</v>
-      </c>
-      <c r="C17" s="9">
-        <v>2003</v>
+        <v>93</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="9" t="s">
+        <v>90</v>
       </c>
       <c r="F17" s="14"/>
     </row>
     <row r="18" spans="1:6" s="8" customFormat="1">
       <c r="A18" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B18" s="9">
-        <v>2004</v>
-      </c>
-      <c r="C18" s="9">
-        <v>2004</v>
+        <v>93</v>
+      </c>
+      <c r="B18" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C18" s="9" t="s">
+        <v>91</v>
       </c>
       <c r="F18" s="14"/>
     </row>
     <row r="19" spans="1:6" s="8" customFormat="1">
       <c r="A19" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="B19" s="9">
-        <v>2005</v>
-      </c>
-      <c r="C19" s="9">
-        <v>2005</v>
+        <v>93</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="C19" s="9" t="s">
+        <v>92</v>
       </c>
       <c r="F19" s="14"/>
     </row>
     <row r="20" spans="1:6" s="8" customFormat="1">
       <c r="A20" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B20" s="9">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="C20" s="9">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="F20" s="14"/>
     </row>
     <row r="21" spans="1:6" s="8" customFormat="1">
       <c r="A21" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B21" s="9">
-        <v>2007</v>
+        <v>2001</v>
       </c>
       <c r="C21" s="9">
-        <v>2007</v>
+        <v>2001</v>
       </c>
       <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" s="8" customFormat="1">
       <c r="A22" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B22" s="9">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="C22" s="9">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" s="8" customFormat="1">
       <c r="A23" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B23" s="9">
-        <v>2009</v>
+        <v>2003</v>
       </c>
       <c r="C23" s="9">
-        <v>2009</v>
+        <v>2003</v>
       </c>
       <c r="F23" s="14"/>
     </row>
     <row r="24" spans="1:6" s="8" customFormat="1">
       <c r="A24" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B24" s="9">
-        <v>2010</v>
+        <v>2004</v>
       </c>
       <c r="C24" s="9">
-        <v>2010</v>
+        <v>2004</v>
       </c>
       <c r="F24" s="14"/>
     </row>
     <row r="25" spans="1:6" s="8" customFormat="1">
       <c r="A25" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B25" s="9">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="C25" s="9">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="F25" s="14"/>
     </row>
     <row r="26" spans="1:6" s="8" customFormat="1">
       <c r="A26" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B26" s="9">
-        <v>2012</v>
+        <v>2006</v>
       </c>
       <c r="C26" s="9">
-        <v>2012</v>
+        <v>2006</v>
       </c>
       <c r="F26" s="14"/>
     </row>
     <row r="27" spans="1:6" s="8" customFormat="1">
       <c r="A27" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B27" s="9">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="C27" s="9">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="F27" s="14"/>
     </row>
     <row r="28" spans="1:6" s="8" customFormat="1">
       <c r="A28" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B28" s="9">
-        <v>2014</v>
+        <v>2008</v>
       </c>
       <c r="C28" s="9">
-        <v>2014</v>
+        <v>2008</v>
       </c>
       <c r="F28" s="14"/>
     </row>
     <row r="29" spans="1:6" s="8" customFormat="1">
       <c r="A29" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B29" s="9">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="C29" s="9">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="F29" s="14"/>
     </row>
     <row r="30" spans="1:6" s="8" customFormat="1">
       <c r="A30" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B30" s="9">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="C30" s="9">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="F30" s="14"/>
     </row>
     <row r="31" spans="1:6" s="8" customFormat="1">
       <c r="A31" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B31" s="9">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="C31" s="9">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="F31" s="14"/>
     </row>
     <row r="32" spans="1:6" s="8" customFormat="1">
       <c r="A32" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B32" s="9">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="C32" s="9">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="F32" s="14"/>
     </row>
     <row r="33" spans="1:6" s="8" customFormat="1">
       <c r="A33" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B33" s="9">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="C33" s="9">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="F33" s="14"/>
     </row>
     <row r="34" spans="1:6" s="8" customFormat="1">
       <c r="A34" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B34" s="9">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="C34" s="9">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="F34" s="14"/>
     </row>
     <row r="35" spans="1:6" s="8" customFormat="1">
       <c r="A35" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B35" s="9">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="C35" s="9">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="F35" s="14"/>
     </row>
     <row r="36" spans="1:6" s="8" customFormat="1">
       <c r="A36" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B36" s="9">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="C36" s="9">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="F36" s="14"/>
     </row>
     <row r="37" spans="1:6" s="8" customFormat="1">
       <c r="A37" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B37" s="9">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="C37" s="9">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="F37" s="14"/>
     </row>
     <row r="38" spans="1:6" s="8" customFormat="1">
       <c r="A38" s="9" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
       <c r="B38" s="9">
+        <v>2018</v>
+      </c>
+      <c r="C38" s="9">
+        <v>2018</v>
+      </c>
+      <c r="F38" s="14"/>
+    </row>
+    <row r="39" spans="1:6" s="8" customFormat="1">
+      <c r="A39" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="9">
+        <v>2019</v>
+      </c>
+      <c r="C39" s="9">
+        <v>2019</v>
+      </c>
+      <c r="F39" s="14"/>
+    </row>
+    <row r="40" spans="1:6" s="8" customFormat="1">
+      <c r="A40" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B40" s="9">
+        <v>2020</v>
+      </c>
+      <c r="C40" s="9">
+        <v>2020</v>
+      </c>
+      <c r="F40" s="14"/>
+    </row>
+    <row r="41" spans="1:6" s="8" customFormat="1">
+      <c r="A41" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B41" s="9">
+        <v>2021</v>
+      </c>
+      <c r="C41" s="9">
+        <v>2021</v>
+      </c>
+      <c r="F41" s="14"/>
+    </row>
+    <row r="42" spans="1:6" s="8" customFormat="1">
+      <c r="A42" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" s="9">
+        <v>2022</v>
+      </c>
+      <c r="C42" s="9">
+        <v>2022</v>
+      </c>
+      <c r="F42" s="14"/>
+    </row>
+    <row r="43" spans="1:6" s="8" customFormat="1">
+      <c r="A43" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="9">
+        <v>2023</v>
+      </c>
+      <c r="C43" s="9">
+        <v>2023</v>
+      </c>
+      <c r="F43" s="14"/>
+    </row>
+    <row r="44" spans="1:6" s="8" customFormat="1">
+      <c r="A44" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="B44" s="9">
         <v>2024</v>
       </c>
-      <c r="C38" s="9">
+      <c r="C44" s="9">
         <v>2024</v>
       </c>
-      <c r="F38" s="14"/>
-    </row>
-    <row r="39" spans="1:6">
-      <c r="A39" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B39" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6">
-      <c r="A40" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B40" t="s">
-        <v>68</v>
-      </c>
-      <c r="C40" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6">
-      <c r="A41" s="3"/>
-    </row>
-    <row r="42" spans="1:6">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
-      <c r="A43" t="s">
-        <v>63</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
-      <c r="A44" t="s">
-        <v>63</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>130</v>
-      </c>
+      <c r="F44" s="14"/>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" t="s">
-        <v>63</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>134</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>134</v>
+      <c r="A45" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B45" t="s">
+        <v>61</v>
+      </c>
+      <c r="C45" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" t="s">
-        <v>63</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>141</v>
+      <c r="A46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B46" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" t="s">
-        <v>63</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>148</v>
-      </c>
+      <c r="A47" s="3"/>
     </row>
     <row r="48" spans="1:6">
       <c r="A48" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>152</v>
+        <v>109</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5">
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:5">
-      <c r="A50" s="3" t="s">
-        <v>64</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" t="s">
+        <v>57</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" t="s">
+        <v>57</v>
       </c>
       <c r="B50" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" t="s">
+        <v>57</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" t="s">
+        <v>57</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" t="s">
+        <v>57</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="B55" s="4"/>
+      <c r="C55" s="4"/>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="D56" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="D57" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="D58" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C59" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D50" t="s">
+      <c r="D59" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="51" spans="1:5">
-      <c r="A51" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="D51" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5">
-      <c r="A52" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B52" s="4" t="s">
+    <row r="60" spans="1:4">
+      <c r="A60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B60" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C60" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D52" t="s">
+      <c r="D60" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="53" spans="1:5">
-      <c r="A53" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B53" s="4" t="s">
+    <row r="61" spans="1:4">
+      <c r="A61" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="D61" t="s">
         <v>127</v>
       </c>
-      <c r="C53" s="4" t="s">
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="D62" t="s">
         <v>127</v>
       </c>
-      <c r="D53" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5">
-      <c r="A54" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="D54" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5">
-      <c r="A55" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B55" s="4" t="s">
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="C55" s="4" t="s">
+      <c r="C63" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D55" t="s">
+      <c r="D63" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="56" spans="1:5">
-      <c r="A56" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B56" s="4" t="s">
+    <row r="64" spans="1:4">
+      <c r="A64" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B64" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="C56" s="4" t="s">
+      <c r="C64" s="4" t="s">
         <v>138</v>
       </c>
-      <c r="D56" t="s">
+      <c r="D64" t="s">
         <v>134</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5">
-      <c r="A57" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="D57" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5">
-      <c r="A58" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>145</v>
-      </c>
-      <c r="D58" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5">
-      <c r="A59" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="D59" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5">
-      <c r="A60" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D60" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5">
-      <c r="A61" s="3"/>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-    </row>
-    <row r="62" spans="1:5">
-      <c r="A62" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B62" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="E62" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5">
-      <c r="A63" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B63" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="C63" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="E63" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5">
-      <c r="A64" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B64" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="E64" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="E65" t="s">
-        <v>135</v>
+        <v>142</v>
+      </c>
+      <c r="D65" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="3" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>121</v>
+        <v>146</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="E66" t="s">
-        <v>120</v>
+        <v>146</v>
+      </c>
+      <c r="D66" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="67" spans="1:5">
-      <c r="A67" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="E67" t="s">
-        <v>120</v>
-      </c>
+      <c r="A67" s="3"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>155</v>
+        <v>125</v>
       </c>
       <c r="E68" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>154</v>
+        <v>126</v>
       </c>
       <c r="E69" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
       <c r="E70" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
       <c r="E71" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>150</v>
+        <v>114</v>
       </c>
       <c r="E72" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>151</v>
+        <v>115</v>
       </c>
       <c r="E73" t="s">
-        <v>149</v>
+        <v>113</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="E74" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="E75" t="s">
-        <v>124</v>
+        <v>146</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="E76" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="E77" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="E78" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E79" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>140</v>
+        <v>118</v>
       </c>
       <c r="E80" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:6">
       <c r="A81" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>139</v>
+        <v>119</v>
       </c>
       <c r="E81" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
     </row>
     <row r="82" spans="1:6">
       <c r="A82" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="E82" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="83" spans="1:6">
       <c r="A83" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="E83" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
     </row>
     <row r="84" spans="1:6">
-      <c r="A84" s="3"/>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
+      <c r="A84" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E84" t="s">
+        <v>138</v>
+      </c>
     </row>
     <row r="85" spans="1:6">
       <c r="A85" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>114</v>
+        <v>139</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F85" t="s">
-        <v>118</v>
+        <v>139</v>
+      </c>
+      <c r="E85" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="86" spans="1:6">
       <c r="A86" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F86" t="s">
-        <v>121</v>
+        <v>133</v>
+      </c>
+      <c r="E86" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="87" spans="1:6">
       <c r="A87" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F87" t="s">
-        <v>125</v>
+        <v>132</v>
+      </c>
+      <c r="E87" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="88" spans="1:6">
       <c r="A88" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F88" t="s">
-        <v>128</v>
+        <v>111</v>
+      </c>
+      <c r="E88" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:6">
       <c r="A89" s="3" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F89" t="s">
-        <v>132</v>
+        <v>112</v>
+      </c>
+      <c r="E89" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B90" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F90" t="s">
-        <v>136</v>
-      </c>
+      <c r="A90" s="3"/>
+      <c r="B90" s="4"/>
+      <c r="C90" s="4"/>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F91" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B92" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C92" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F92" t="s">
         <v>114</v>
-      </c>
-      <c r="C92" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="F92" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:6">
       <c r="A93" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F93" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F94" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
     </row>
     <row r="95" spans="1:6">
       <c r="A95" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F95" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
     </row>
     <row r="96" spans="1:6">
       <c r="A96" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F96" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="97" spans="1:6">
       <c r="A97" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B97" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F97" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="98" spans="1:6">
       <c r="A98" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F98" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="99" spans="1:6">
       <c r="A99" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F99" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="100" spans="1:6">
       <c r="A100" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F100" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:6">
       <c r="A101" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="F101" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="102" spans="1:6">
       <c r="A102" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F102" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B103" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C103" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F103" t="s">
         <v>115</v>
-      </c>
-      <c r="C103" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="F103" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="104" spans="1:6">
       <c r="A104" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F104" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="105" spans="1:6">
       <c r="A105" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F105" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
     </row>
     <row r="106" spans="1:6">
       <c r="A106" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F106" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
     </row>
     <row r="107" spans="1:6">
-      <c r="A107" s="3"/>
-      <c r="B107" s="4"/>
-      <c r="C107" s="4"/>
+      <c r="A107" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B107" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C107" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F107" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="108" spans="1:6">
       <c r="A108" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B108" s="4">
-        <v>301</v>
-      </c>
-      <c r="C108" s="4">
-        <v>301</v>
+        <v>63</v>
+      </c>
+      <c r="B108" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C108" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F108" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
     </row>
     <row r="109" spans="1:6">
       <c r="A109" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B109" s="4">
-        <v>302</v>
-      </c>
-      <c r="C109" s="4">
-        <v>302</v>
+        <v>63</v>
+      </c>
+      <c r="B109" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C109" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F109" t="s">
-        <v>121</v>
+        <v>137</v>
       </c>
     </row>
     <row r="110" spans="1:6">
       <c r="A110" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B110" s="4">
-        <v>303</v>
-      </c>
-      <c r="C110" s="4">
-        <v>303</v>
+        <v>63</v>
+      </c>
+      <c r="B110" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C110" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F110" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="111" spans="1:6">
       <c r="A111" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B111" s="4">
-        <v>304</v>
-      </c>
-      <c r="C111" s="4">
-        <v>304</v>
+        <v>63</v>
+      </c>
+      <c r="B111" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C111" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F111" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
     </row>
     <row r="112" spans="1:6">
       <c r="A112" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B112" s="4">
-        <v>305</v>
-      </c>
-      <c r="C112" s="4">
-        <v>305</v>
+        <v>63</v>
+      </c>
+      <c r="B112" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C112" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F112" t="s">
-        <v>132</v>
+        <v>148</v>
       </c>
     </row>
     <row r="113" spans="1:6">
-      <c r="A113" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B113" s="4">
-        <v>306</v>
-      </c>
-      <c r="C113" s="4">
-        <v>306</v>
-      </c>
-      <c r="F113" t="s">
-        <v>136</v>
-      </c>
+      <c r="A113" s="3"/>
+      <c r="B113" s="4"/>
+      <c r="C113" s="4"/>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B114" s="4">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="C114" s="4">
-        <v>307</v>
+        <v>301</v>
       </c>
       <c r="F114" t="s">
-        <v>139</v>
+        <v>111</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B115" s="4">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="C115" s="4">
-        <v>308</v>
+        <v>302</v>
       </c>
       <c r="F115" t="s">
-        <v>143</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B116" s="4">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="C116" s="4">
-        <v>309</v>
+        <v>303</v>
       </c>
       <c r="F116" t="s">
-        <v>146</v>
+        <v>118</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B117" s="4">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="C117" s="4">
-        <v>310</v>
+        <v>304</v>
       </c>
       <c r="F117" t="s">
-        <v>150</v>
+        <v>121</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B118" s="4">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="C118" s="4">
-        <v>311</v>
+        <v>305</v>
       </c>
       <c r="F118" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B119" s="4">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="C119" s="4">
-        <v>312</v>
+        <v>306</v>
       </c>
       <c r="F119" t="s">
-        <v>119</v>
+        <v>129</v>
       </c>
     </row>
     <row r="120" spans="1:6">
       <c r="A120" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B120" s="4">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="C120" s="4">
-        <v>313</v>
+        <v>307</v>
       </c>
       <c r="F120" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
     </row>
     <row r="121" spans="1:6">
       <c r="A121" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B121" s="4">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="C121" s="4">
-        <v>314</v>
+        <v>308</v>
       </c>
       <c r="F121" t="s">
-        <v>126</v>
+        <v>136</v>
       </c>
     </row>
     <row r="122" spans="1:6">
       <c r="A122" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B122" s="4">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="C122" s="4">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="F122" t="s">
-        <v>129</v>
+        <v>139</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B123" s="4">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="C123" s="4">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="F123" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
     </row>
     <row r="124" spans="1:6">
       <c r="A124" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B124" s="4">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="C124" s="4">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="F124" t="s">
-        <v>137</v>
+        <v>147</v>
       </c>
     </row>
     <row r="125" spans="1:6">
       <c r="A125" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B125" s="4">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="C125" s="4">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="F125" t="s">
-        <v>140</v>
+        <v>112</v>
       </c>
     </row>
     <row r="126" spans="1:6">
       <c r="A126" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B126" s="4">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C126" s="4">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="F126" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
     </row>
     <row r="127" spans="1:6">
       <c r="A127" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B127" s="4">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="C127" s="4">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="F127" t="s">
-        <v>147</v>
+        <v>119</v>
       </c>
     </row>
     <row r="128" spans="1:6">
       <c r="A128" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B128" s="4">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="C128" s="4">
-        <v>321</v>
+        <v>315</v>
       </c>
       <c r="F128" t="s">
-        <v>151</v>
+        <v>122</v>
       </c>
     </row>
     <row r="129" spans="1:6">
       <c r="A129" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B129" s="4">
+        <v>316</v>
+      </c>
+      <c r="C129" s="4">
+        <v>316</v>
+      </c>
+      <c r="F129" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6">
+      <c r="A130" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B130" s="4">
+        <v>317</v>
+      </c>
+      <c r="C130" s="4">
+        <v>317</v>
+      </c>
+      <c r="F130" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="131" spans="1:6">
+      <c r="A131" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B131" s="4">
+        <v>318</v>
+      </c>
+      <c r="C131" s="4">
+        <v>318</v>
+      </c>
+      <c r="F131" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6">
+      <c r="A132" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B132" s="4">
+        <v>319</v>
+      </c>
+      <c r="C132" s="4">
+        <v>319</v>
+      </c>
+      <c r="F132" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6">
+      <c r="A133" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B133" s="4">
+        <v>320</v>
+      </c>
+      <c r="C133" s="4">
+        <v>320</v>
+      </c>
+      <c r="F133" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6">
+      <c r="A134" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B134" s="4">
+        <v>321</v>
+      </c>
+      <c r="C134" s="4">
+        <v>321</v>
+      </c>
+      <c r="F134" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6">
+      <c r="A135" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B135" s="4">
         <v>322</v>
       </c>
-      <c r="C129" s="4">
+      <c r="C135" s="4">
         <v>322</v>
       </c>
-      <c r="F129" t="s">
-        <v>155</v>
+      <c r="F135" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A245:C290">
-    <sortCondition ref="B245:B290"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A251:C296">
+    <sortCondition ref="B251:B296"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3101,7 +3175,7 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -3114,30 +3188,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="6" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>113</v>
+        <v>151</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -3168,37 +3242,37 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" s="12" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B1" s="12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C1" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="H1" s="12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="J1" s="12" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="K1" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="M1" s="10" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="N1" s="12" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:14">
@@ -3206,34 +3280,34 @@
         <v>1</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F2">
         <v>301</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="J2" s="13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K2" s="11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="M2" s="11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -3241,34 +3315,34 @@
         <v>2</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="E3" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F3">
         <v>302</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="J3" s="13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="N3" s="18" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -3276,34 +3350,34 @@
         <v>3</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F4">
         <v>303</v>
       </c>
       <c r="H4" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="J4" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="M4" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="N4" s="18" t="s">
         <v>130</v>
-      </c>
-      <c r="J4" s="13" t="s">
-        <v>123</v>
-      </c>
-      <c r="K4" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="M4" s="13" t="s">
-        <v>135</v>
-      </c>
-      <c r="N4" s="18" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -3311,34 +3385,34 @@
         <v>4</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F5">
         <v>304</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="J5" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="M5" s="13" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="N5" s="18" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -3346,34 +3420,34 @@
         <v>5</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F6">
         <v>305</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="N6" s="18" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -3381,34 +3455,34 @@
         <v>6</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="E7" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F7">
         <v>306</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="K7" s="13" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="M7" s="11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="N7" s="18" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -3416,34 +3490,34 @@
         <v>7</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F8">
         <v>307</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="M8" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="N8" s="18" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -3451,31 +3525,31 @@
         <v>8</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F9">
         <v>308</v>
       </c>
       <c r="J9" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="K9" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="M9" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="N9" s="18" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -3483,31 +3557,31 @@
         <v>9</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F10">
         <v>309</v>
       </c>
       <c r="J10" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="M10" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="N10" s="18" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="11" spans="1:14">
@@ -3515,31 +3589,31 @@
         <v>10</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F11">
         <v>310</v>
       </c>
       <c r="J11" s="13" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="K11" s="13" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="M11" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="N11" s="18" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -3547,31 +3621,31 @@
         <v>11</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="F12">
         <v>311</v>
       </c>
       <c r="J12" s="13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="K12" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="N12" s="18" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:14">
@@ -3579,25 +3653,25 @@
         <v>1</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F13">
         <v>312</v>
       </c>
       <c r="M13" s="13" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="N13" s="18" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:14">
@@ -3605,25 +3679,25 @@
         <v>2</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F14">
         <v>313</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="N14" s="18" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:14">
@@ -3631,25 +3705,25 @@
         <v>3</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F15">
         <v>314</v>
       </c>
       <c r="M15" s="11" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="N15" s="18" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="16" spans="1:14">
@@ -3657,25 +3731,25 @@
         <v>4</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F16">
         <v>315</v>
       </c>
       <c r="M16" s="11" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="N16" s="18" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:14">
@@ -3683,25 +3757,25 @@
         <v>5</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F17">
         <v>316</v>
       </c>
       <c r="M17" s="11" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="N17" s="18" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="18" spans="1:14">
@@ -3709,25 +3783,25 @@
         <v>6</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F18">
         <v>317</v>
       </c>
       <c r="M18" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="N18" s="18" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="19" spans="1:14">
@@ -3735,25 +3809,25 @@
         <v>7</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="E19" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F19">
         <v>318</v>
       </c>
       <c r="M19" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="N19" s="18" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="20" spans="1:14">
@@ -3761,25 +3835,25 @@
         <v>8</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E20" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F20">
         <v>319</v>
       </c>
       <c r="M20" s="13" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="N20" s="18" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:14">
@@ -3787,25 +3861,25 @@
         <v>9</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="E21" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F21">
         <v>320</v>
       </c>
       <c r="M21" s="13" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="N21" s="18" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:14">
@@ -3813,25 +3887,25 @@
         <v>10</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F22">
         <v>321</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="N22" s="18" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="1:14">
@@ -3839,25 +3913,25 @@
         <v>11</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="E23" s="13" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="F23">
         <v>322</v>
       </c>
       <c r="M23" s="11" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="N23" s="18" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ng: update pretas site
</commit_message>
<xml_diff>
--- a/LF/PreTAS/Nigeria/apri 2024/ng_lf_pretas_202404_1_site.xlsx
+++ b/LF/PreTAS/Nigeria/apri 2024/ng_lf_pretas_202404_1_site.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\PreTAS\Nigeria\apri 2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69EBE882-FDCF-4433-8D94-F59227C7E7FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E0D0539-571D-462C-B52E-16CC313ABA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="687" uniqueCount="166">
   <si>
     <t>type</t>
   </si>
@@ -488,12 +488,6 @@
     <t>Code Site</t>
   </si>
   <si>
-    <t>(Apr 2024) - 1. Nigeria - Pre TAS LF Site Form V2</t>
-  </si>
-  <si>
-    <t>ng_lf_pretas_202404_1_site_v2</t>
-  </si>
-  <si>
     <t>team</t>
   </si>
   <si>
@@ -525,13 +519,28 @@
   </si>
   <si>
     <t>Select the community type</t>
+  </si>
+  <si>
+    <t>Birnin Kebbi</t>
+  </si>
+  <si>
+    <t>Kardi</t>
+  </si>
+  <si>
+    <t>Gwadangaji</t>
+  </si>
+  <si>
+    <t>(Apr 2024) - 1. Nigeria - Pre TAS LF Site Form V3</t>
+  </si>
+  <si>
+    <t>ng_lf_pretas_202404_1_site_v3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -590,6 +599,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -641,7 +656,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -692,6 +707,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -980,11 +996,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C6" sqref="C6"/>
+      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1048,7 +1064,7 @@
     </row>
     <row r="2" spans="1:13" s="9" customFormat="1" ht="47.25">
       <c r="A2" s="9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B2" s="14" t="s">
         <v>14</v>
@@ -1120,7 +1136,7 @@
         <v>25</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D5" s="14"/>
       <c r="G5" s="14"/>
@@ -1143,7 +1159,7 @@
         <v>28</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D6" s="14"/>
       <c r="G6" s="14"/>
@@ -1195,7 +1211,7 @@
         <v>36</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="14"/>
@@ -1218,7 +1234,7 @@
         <v>38</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D9" s="14"/>
       <c r="J9" s="14" t="s">
@@ -1423,11 +1439,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:F135"/>
+  <dimension ref="A1:F142"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A6:XFD11"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A140" sqref="A140:A142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1459,57 +1475,57 @@
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1">
       <c r="A2" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1">
       <c r="A3" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B3" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B3" s="19" t="s">
-        <v>154</v>
-      </c>
       <c r="C3" s="19" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:6" s="4" customFormat="1">
       <c r="A4" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:6" s="4" customFormat="1">
       <c r="A5" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="4" customFormat="1">
       <c r="A6" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="8" customFormat="1">
@@ -2073,10 +2089,10 @@
         <v>58</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>113</v>
+        <v>161</v>
       </c>
       <c r="D56" t="s">
         <v>109</v>
@@ -2087,10 +2103,10 @@
         <v>58</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D57" t="s">
         <v>109</v>
@@ -2101,13 +2117,13 @@
         <v>58</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="D58" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="59" spans="1:4">
@@ -2115,10 +2131,10 @@
         <v>58</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D59" t="s">
         <v>116</v>
@@ -2129,13 +2145,13 @@
         <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D60" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:4">
@@ -2143,13 +2159,13 @@
         <v>58</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="D61" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -2157,10 +2173,10 @@
         <v>58</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D62" t="s">
         <v>127</v>
@@ -2171,13 +2187,13 @@
         <v>58</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D63" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="64" spans="1:4">
@@ -2185,10 +2201,10 @@
         <v>58</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="D64" t="s">
         <v>134</v>
@@ -2199,13 +2215,13 @@
         <v>58</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D65" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -2213,43 +2229,43 @@
         <v>58</v>
       </c>
       <c r="B66" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D66" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B67" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C67" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="D66" t="s">
+      <c r="D67" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="67" spans="1:5">
-      <c r="A67" s="3"/>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-    </row>
     <row r="68" spans="1:5">
-      <c r="A68" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E68" t="s">
-        <v>124</v>
-      </c>
+      <c r="A68" s="3"/>
+      <c r="B68" s="4"/>
+      <c r="C68" s="4"/>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="3" t="s">
         <v>59</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E69" t="s">
         <v>124</v>
@@ -2260,41 +2276,41 @@
         <v>59</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E70" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B71" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="E71" t="s">
-        <v>128</v>
+      <c r="B71" t="s">
+        <v>163</v>
+      </c>
+      <c r="C71" t="s">
+        <v>163</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B72" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="C72" s="4" t="s">
-        <v>114</v>
-      </c>
-      <c r="E72" t="s">
-        <v>113</v>
+      <c r="B72" t="s">
+        <v>162</v>
+      </c>
+      <c r="C72" t="s">
+        <v>162</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2302,13 +2318,13 @@
         <v>59</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="E73" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2316,13 +2332,13 @@
         <v>59</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>148</v>
+        <v>129</v>
       </c>
       <c r="E74" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2330,13 +2346,13 @@
         <v>59</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>147</v>
+        <v>114</v>
       </c>
       <c r="E75" t="s">
-        <v>146</v>
+        <v>113</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2344,13 +2360,13 @@
         <v>59</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="E76" t="s">
-        <v>135</v>
+        <v>113</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2358,13 +2374,13 @@
         <v>59</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>136</v>
+        <v>148</v>
       </c>
       <c r="E77" t="s">
-        <v>135</v>
+        <v>146</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2372,13 +2388,13 @@
         <v>59</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
       <c r="E78" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2386,13 +2402,13 @@
         <v>59</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="E79" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2400,13 +2416,13 @@
         <v>59</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>118</v>
+        <v>136</v>
       </c>
       <c r="E80" t="s">
-        <v>117</v>
+        <v>135</v>
       </c>
     </row>
     <row r="81" spans="1:6">
@@ -2414,13 +2430,13 @@
         <v>59</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>119</v>
+        <v>143</v>
       </c>
       <c r="E81" t="s">
-        <v>117</v>
+        <v>142</v>
       </c>
     </row>
     <row r="82" spans="1:6">
@@ -2428,13 +2444,13 @@
         <v>59</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>122</v>
+        <v>144</v>
       </c>
       <c r="E82" t="s">
-        <v>120</v>
+        <v>142</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2442,13 +2458,13 @@
         <v>59</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="E83" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2456,13 +2472,13 @@
         <v>59</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="E84" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
     </row>
     <row r="85" spans="1:6">
@@ -2470,13 +2486,13 @@
         <v>59</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="E85" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2484,13 +2500,13 @@
         <v>59</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="E86" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="87" spans="1:6">
@@ -2498,13 +2514,13 @@
         <v>59</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>132</v>
+        <v>140</v>
       </c>
       <c r="E87" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2512,13 +2528,13 @@
         <v>59</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>111</v>
+        <v>139</v>
       </c>
       <c r="E88" t="s">
-        <v>110</v>
+        <v>138</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2526,61 +2542,61 @@
         <v>59</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="E89" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
     </row>
     <row r="90" spans="1:6">
-      <c r="A90" s="3"/>
-      <c r="B90" s="4"/>
-      <c r="C90" s="4"/>
+      <c r="A90" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B90" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="C90" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E90" t="s">
+        <v>131</v>
+      </c>
     </row>
     <row r="91" spans="1:6">
       <c r="A91" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F91" t="s">
         <v>111</v>
+      </c>
+      <c r="E91" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="1:6">
       <c r="A92" s="3" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F92" t="s">
-        <v>114</v>
+        <v>112</v>
+      </c>
+      <c r="E92" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:6">
-      <c r="A93" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B93" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="F93" t="s">
-        <v>118</v>
-      </c>
+      <c r="A93" s="3"/>
+      <c r="B93" s="4"/>
+      <c r="C93" s="4"/>
     </row>
     <row r="94" spans="1:6">
       <c r="A94" s="3" t="s">
@@ -2593,7 +2609,7 @@
         <v>107</v>
       </c>
       <c r="F94" t="s">
-        <v>121</v>
+        <v>111</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -2607,7 +2623,7 @@
         <v>107</v>
       </c>
       <c r="F95" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -2621,7 +2637,7 @@
         <v>107</v>
       </c>
       <c r="F96" t="s">
-        <v>129</v>
+        <v>118</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -2635,7 +2651,7 @@
         <v>107</v>
       </c>
       <c r="F97" t="s">
-        <v>132</v>
+        <v>121</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -2649,7 +2665,7 @@
         <v>107</v>
       </c>
       <c r="F98" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -2663,7 +2679,7 @@
         <v>107</v>
       </c>
       <c r="F99" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -2677,7 +2693,7 @@
         <v>107</v>
       </c>
       <c r="F100" t="s">
-        <v>143</v>
+        <v>132</v>
       </c>
     </row>
     <row r="101" spans="1:6">
@@ -2691,7 +2707,7 @@
         <v>107</v>
       </c>
       <c r="F101" t="s">
-        <v>147</v>
+        <v>136</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -2699,13 +2715,13 @@
         <v>63</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F102" t="s">
-        <v>112</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="1:6">
@@ -2713,13 +2729,13 @@
         <v>63</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F103" t="s">
-        <v>115</v>
+        <v>143</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -2727,13 +2743,13 @@
         <v>63</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F104" t="s">
-        <v>119</v>
+        <v>147</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -2747,7 +2763,7 @@
         <v>108</v>
       </c>
       <c r="F105" t="s">
-        <v>122</v>
+        <v>112</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -2761,7 +2777,7 @@
         <v>108</v>
       </c>
       <c r="F106" t="s">
-        <v>126</v>
+        <v>115</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -2775,7 +2791,7 @@
         <v>108</v>
       </c>
       <c r="F107" t="s">
-        <v>130</v>
+        <v>119</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -2789,7 +2805,7 @@
         <v>108</v>
       </c>
       <c r="F108" t="s">
-        <v>133</v>
+        <v>122</v>
       </c>
     </row>
     <row r="109" spans="1:6">
@@ -2803,7 +2819,7 @@
         <v>108</v>
       </c>
       <c r="F109" t="s">
-        <v>137</v>
+        <v>126</v>
       </c>
     </row>
     <row r="110" spans="1:6">
@@ -2817,7 +2833,7 @@
         <v>108</v>
       </c>
       <c r="F110" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -2831,7 +2847,7 @@
         <v>108</v>
       </c>
       <c r="F111" t="s">
-        <v>144</v>
+        <v>133</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -2845,96 +2861,96 @@
         <v>108</v>
       </c>
       <c r="F112" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="113" spans="1:6">
-      <c r="A113" s="3"/>
-      <c r="B113" s="4"/>
-      <c r="C113" s="4"/>
+      <c r="A113" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B113" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C113" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="F113" t="s">
+        <v>140</v>
+      </c>
     </row>
     <row r="114" spans="1:6">
       <c r="A114" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B114" s="4">
-        <v>301</v>
-      </c>
-      <c r="C114" s="4">
-        <v>301</v>
+        <v>63</v>
+      </c>
+      <c r="B114" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C114" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F114" t="s">
-        <v>111</v>
+        <v>144</v>
       </c>
     </row>
     <row r="115" spans="1:6">
       <c r="A115" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B115" s="4">
-        <v>302</v>
-      </c>
-      <c r="C115" s="4">
-        <v>302</v>
+        <v>63</v>
+      </c>
+      <c r="B115" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C115" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F115" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
     </row>
     <row r="116" spans="1:6">
       <c r="A116" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B116" s="4">
-        <v>303</v>
-      </c>
-      <c r="C116" s="4">
-        <v>303</v>
+        <v>63</v>
+      </c>
+      <c r="B116" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C116" s="4" t="s">
+        <v>107</v>
       </c>
       <c r="F116" t="s">
-        <v>118</v>
+        <v>162</v>
       </c>
     </row>
     <row r="117" spans="1:6">
       <c r="A117" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B117" s="4">
-        <v>304</v>
-      </c>
-      <c r="C117" s="4">
-        <v>304</v>
+        <v>63</v>
+      </c>
+      <c r="B117" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C117" s="4" t="s">
+        <v>108</v>
       </c>
       <c r="F117" t="s">
-        <v>121</v>
+        <v>163</v>
       </c>
     </row>
     <row r="118" spans="1:6">
-      <c r="A118" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B118" s="4">
-        <v>305</v>
-      </c>
-      <c r="C118" s="4">
-        <v>305</v>
-      </c>
-      <c r="F118" t="s">
-        <v>125</v>
-      </c>
+      <c r="A118" s="3"/>
+      <c r="B118" s="4"/>
+      <c r="C118" s="4"/>
     </row>
     <row r="119" spans="1:6">
       <c r="A119" s="3" t="s">
         <v>64</v>
       </c>
       <c r="B119" s="4">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="C119" s="4">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="F119" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -2942,13 +2958,13 @@
         <v>64</v>
       </c>
       <c r="B120" s="4">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="C120" s="4">
-        <v>307</v>
+        <v>302</v>
       </c>
       <c r="F120" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -2956,13 +2972,13 @@
         <v>64</v>
       </c>
       <c r="B121" s="4">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="C121" s="4">
-        <v>308</v>
+        <v>303</v>
       </c>
       <c r="F121" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -2970,13 +2986,13 @@
         <v>64</v>
       </c>
       <c r="B122" s="4">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="C122" s="4">
-        <v>309</v>
+        <v>304</v>
       </c>
       <c r="F122" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="123" spans="1:6">
@@ -2984,13 +3000,13 @@
         <v>64</v>
       </c>
       <c r="B123" s="4">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="C123" s="4">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="F123" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -2998,13 +3014,13 @@
         <v>64</v>
       </c>
       <c r="B124" s="4">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C124" s="4">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="F124" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3012,13 +3028,13 @@
         <v>64</v>
       </c>
       <c r="B125" s="4">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="C125" s="4">
-        <v>312</v>
+        <v>307</v>
       </c>
       <c r="F125" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3026,13 +3042,13 @@
         <v>64</v>
       </c>
       <c r="B126" s="4">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="C126" s="4">
-        <v>313</v>
+        <v>308</v>
       </c>
       <c r="F126" t="s">
-        <v>115</v>
+        <v>136</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3040,13 +3056,13 @@
         <v>64</v>
       </c>
       <c r="B127" s="4">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="C127" s="4">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="F127" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3054,13 +3070,13 @@
         <v>64</v>
       </c>
       <c r="B128" s="4">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="C128" s="4">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="F128" t="s">
-        <v>122</v>
+        <v>143</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3068,13 +3084,13 @@
         <v>64</v>
       </c>
       <c r="B129" s="4">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="C129" s="4">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="F129" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3082,13 +3098,13 @@
         <v>64</v>
       </c>
       <c r="B130" s="4">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="C130" s="4">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="F130" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3096,13 +3112,13 @@
         <v>64</v>
       </c>
       <c r="B131" s="4">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="C131" s="4">
-        <v>318</v>
+        <v>313</v>
       </c>
       <c r="F131" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="1:6">
@@ -3110,13 +3126,13 @@
         <v>64</v>
       </c>
       <c r="B132" s="4">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="C132" s="4">
-        <v>319</v>
+        <v>314</v>
       </c>
       <c r="F132" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="133" spans="1:6">
@@ -3124,13 +3140,13 @@
         <v>64</v>
       </c>
       <c r="B133" s="4">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="C133" s="4">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="F133" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="134" spans="1:6">
@@ -3138,13 +3154,13 @@
         <v>64</v>
       </c>
       <c r="B134" s="4">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C134" s="4">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="F134" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="135" spans="1:6">
@@ -3152,18 +3168,117 @@
         <v>64</v>
       </c>
       <c r="B135" s="4">
+        <v>317</v>
+      </c>
+      <c r="C135" s="4">
+        <v>317</v>
+      </c>
+      <c r="F135" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6">
+      <c r="A136" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B136" s="4">
+        <v>318</v>
+      </c>
+      <c r="C136" s="4">
+        <v>318</v>
+      </c>
+      <c r="F136" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6">
+      <c r="A137" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B137" s="4">
+        <v>319</v>
+      </c>
+      <c r="C137" s="4">
+        <v>319</v>
+      </c>
+      <c r="F137" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6">
+      <c r="A138" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B138" s="4">
+        <v>320</v>
+      </c>
+      <c r="C138" s="4">
+        <v>320</v>
+      </c>
+      <c r="F138" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6">
+      <c r="A139" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B139" s="4">
+        <v>321</v>
+      </c>
+      <c r="C139" s="4">
+        <v>321</v>
+      </c>
+      <c r="F139" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6">
+      <c r="A140" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B140" s="4">
         <v>322</v>
       </c>
-      <c r="C135" s="4">
+      <c r="C140" s="4">
         <v>322</v>
       </c>
-      <c r="F135" t="s">
+      <c r="F140" t="s">
         <v>148</v>
       </c>
     </row>
+    <row r="141" spans="1:6">
+      <c r="A141" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B141">
+        <v>323</v>
+      </c>
+      <c r="C141">
+        <v>323</v>
+      </c>
+      <c r="F141" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6">
+      <c r="A142" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B142">
+        <v>324</v>
+      </c>
+      <c r="C142">
+        <v>324</v>
+      </c>
+      <c r="F142" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A251:C296">
-    <sortCondition ref="B251:B296"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A69:E92">
+    <sortCondition ref="E69:E92"/>
+    <sortCondition ref="B69:B92"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -3174,7 +3289,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -3202,10 +3317,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="9" t="s">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="C2" s="8" t="s">
         <v>69</v>
@@ -3222,10 +3337,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8701DA20-CB5E-4F2E-9F23-E54B3FF53026}">
-  <dimension ref="A1:N23"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D23"/>
+      <selection activeCell="F24" sqref="F24:F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -3934,6 +4049,40 @@
         <v>112</v>
       </c>
     </row>
+    <row r="24" spans="1:14">
+      <c r="B24" t="s">
+        <v>109</v>
+      </c>
+      <c r="C24" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D24" t="s">
+        <v>162</v>
+      </c>
+      <c r="E24" t="s">
+        <v>107</v>
+      </c>
+      <c r="F24">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="B25" t="s">
+        <v>109</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="D25" t="s">
+        <v>163</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F25">
+        <v>324</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M2:N23">
     <sortCondition ref="M2:M23"/>

</xml_diff>